<commit_message>
Grafik dah di sediakan
</commit_message>
<xml_diff>
--- a/TA bab 1-4/uji 100x -300x all.xlsx
+++ b/TA bab 1-4/uji 100x -300x all.xlsx
@@ -192,7 +192,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$4</c:f>
+              <c:f>Sheet1!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -215,7 +215,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$14</c:f>
+              <c:f>Sheet1!$B$5:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -254,7 +254,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$14</c:f>
+              <c:f>Sheet1!$C$5:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -303,7 +303,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$4</c:f>
+              <c:f>Sheet1!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -326,7 +326,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$14</c:f>
+              <c:f>Sheet1!$B$5:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -365,7 +365,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$14</c:f>
+              <c:f>Sheet1!$D$5:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -414,7 +414,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$4</c:f>
+              <c:f>Sheet1!$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -437,7 +437,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$14</c:f>
+              <c:f>Sheet1!$B$5:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -476,7 +476,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$5:$F$14</c:f>
+              <c:f>Sheet1!$E$5:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -521,7 +521,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -920,7 +919,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$4</c:f>
+              <c:f>Sheet1!$H$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -943,7 +942,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$5:$H$14</c:f>
+              <c:f>Sheet1!$G$5:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -982,7 +981,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$5:$I$14</c:f>
+              <c:f>Sheet1!$H$5:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1031,7 +1030,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$4</c:f>
+              <c:f>Sheet1!$I$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1054,7 +1053,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$5:$H$14</c:f>
+              <c:f>Sheet1!$G$5:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1093,7 +1092,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$5:$J$14</c:f>
+              <c:f>Sheet1!$I$5:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1142,7 +1141,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$4</c:f>
+              <c:f>Sheet1!$J$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1165,7 +1164,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$5:$H$14</c:f>
+              <c:f>Sheet1!$G$5:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1204,7 +1203,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$5:$K$14</c:f>
+              <c:f>Sheet1!$J$5:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1637,7 +1636,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$4</c:f>
+              <c:f>Sheet1!$M$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1660,7 +1659,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$M$5:$M$14</c:f>
+              <c:f>Sheet1!$L$5:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1699,7 +1698,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$5:$N$14</c:f>
+              <c:f>Sheet1!$M$5:$M$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1748,7 +1747,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$4</c:f>
+              <c:f>Sheet1!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1771,7 +1770,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$M$5:$M$14</c:f>
+              <c:f>Sheet1!$L$5:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1810,7 +1809,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$5:$O$14</c:f>
+              <c:f>Sheet1!$N$5:$N$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1859,7 +1858,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$4</c:f>
+              <c:f>Sheet1!$O$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1882,7 +1881,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$M$5:$M$14</c:f>
+              <c:f>Sheet1!$L$5:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1921,7 +1920,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$5:$P$14</c:f>
+              <c:f>Sheet1!$O$5:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2354,7 +2353,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$4</c:f>
+              <c:f>Sheet1!$R$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2377,7 +2376,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$R$5:$R$14</c:f>
+              <c:f>Sheet1!$Q$5:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2416,7 +2415,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$5:$S$14</c:f>
+              <c:f>Sheet1!$R$5:$R$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2465,7 +2464,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$4</c:f>
+              <c:f>Sheet1!$S$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2488,7 +2487,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$R$5:$R$14</c:f>
+              <c:f>Sheet1!$Q$5:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2527,7 +2526,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$5:$T$14</c:f>
+              <c:f>Sheet1!$S$5:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2576,7 +2575,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$4</c:f>
+              <c:f>Sheet1!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2599,7 +2598,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$R$5:$R$14</c:f>
+              <c:f>Sheet1!$Q$5:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2638,7 +2637,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$5:$U$14</c:f>
+              <c:f>Sheet1!$T$5:$T$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3076,7 +3075,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$X$4</c:f>
+              <c:f>Sheet1!$W$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3099,7 +3098,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$W$5:$W$14</c:f>
+              <c:f>Sheet1!$V$5:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3138,7 +3137,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$X$5:$X$14</c:f>
+              <c:f>Sheet1!$W$5:$W$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3187,7 +3186,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$4</c:f>
+              <c:f>Sheet1!$X$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3210,7 +3209,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$W$5:$W$14</c:f>
+              <c:f>Sheet1!$V$5:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3249,7 +3248,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Y$5:$Y$14</c:f>
+              <c:f>Sheet1!$X$5:$X$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3298,7 +3297,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Z$4</c:f>
+              <c:f>Sheet1!$Y$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3321,7 +3320,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$W$5:$W$14</c:f>
+              <c:f>Sheet1!$V$5:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3360,7 +3359,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Z$5:$Z$14</c:f>
+              <c:f>Sheet1!$Y$5:$Y$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3793,7 +3792,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AC$4</c:f>
+              <c:f>Sheet1!$AB$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3816,78 +3815,78 @@
           </c:marker>
           <c:cat>
             <c:numRef>
+              <c:f>Sheet1!$AA$5:$AA$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>Sheet1!$AB$5:$AB$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1960.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>482.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>425.39</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>312.47000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1580.17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>418.52</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>202.64</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>790.17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>1828.27</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$AC$5:$AC$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>682.19</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>382.61</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>698.65</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>747.69</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1491.12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1910.56</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>574.52</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1145.46</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1987.18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>907.07</c:v>
+                  <c:v>1347.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3904,7 +3903,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AD$4</c:f>
+              <c:f>Sheet1!$AC$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3927,7 +3926,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$AB$5:$AB$14</c:f>
+              <c:f>Sheet1!$AA$5:$AA$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3966,39 +3965,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AD$5:$AD$14</c:f>
+              <c:f>Sheet1!$AC$5:$AC$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>849</c:v>
+                  <c:v>796.96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1175</c:v>
+                  <c:v>844</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1052.3599999999999</c:v>
+                  <c:v>516.21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1337.06</c:v>
+                  <c:v>1276.6300000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1368.43</c:v>
+                  <c:v>1469.02</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>414.36</c:v>
+                  <c:v>622.44000000000096</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1155.45</c:v>
+                  <c:v>1067</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1286</c:v>
+                  <c:v>1581.79</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1056.45</c:v>
+                  <c:v>1443.65</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1262.81</c:v>
+                  <c:v>1057</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4015,7 +4014,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AE$4</c:f>
+              <c:f>Sheet1!$AD$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4038,7 +4037,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$AB$5:$AB$14</c:f>
+              <c:f>Sheet1!$AA$5:$AA$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4077,39 +4076,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AE$5:$AE$14</c:f>
+              <c:f>Sheet1!$AD$5:$AD$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1934.74</c:v>
+                  <c:v>1196.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2055.98</c:v>
+                  <c:v>2293.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1778.74</c:v>
+                  <c:v>2621.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1470.48</c:v>
+                  <c:v>2020.11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1047.07</c:v>
+                  <c:v>800.56</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1588.11</c:v>
+                  <c:v>2548.67</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2057.0100000000002</c:v>
+                  <c:v>2644.39</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1499.76</c:v>
+                  <c:v>1310.33</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>937.93</c:v>
+                  <c:v>334.67</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1588.05</c:v>
+                  <c:v>1169.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7769,13 +7768,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -7799,13 +7798,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>595312</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>290512</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -7829,13 +7828,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -7859,13 +7858,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -7889,13 +7888,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -7919,13 +7918,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -8213,857 +8212,857 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:AE14"/>
+  <dimension ref="B2:AD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="W2" t="s">
+      <c r="V2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="M3" t="s">
+      <c r="L3" t="s">
         <v>1</v>
       </c>
-      <c r="R3" t="s">
+      <c r="Q3" t="s">
         <v>5</v>
       </c>
-      <c r="W3" t="s">
+      <c r="V3" t="s">
         <v>1</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AA3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
       <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" t="s">
+        <v>8</v>
+      </c>
+      <c r="W4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>15.492957746478901</v>
+      </c>
+      <c r="D5">
+        <v>14.6666666666667</v>
+      </c>
+      <c r="E5">
+        <v>29.268292682926798</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>404.72</v>
+      </c>
+      <c r="I5">
+        <v>1163.02</v>
+      </c>
+      <c r="J5">
+        <v>2007.96</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>17.741935483871</v>
+      </c>
+      <c r="N5">
+        <v>11.5942028985507</v>
+      </c>
+      <c r="O5">
+        <v>35.064935064935099</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>682.19</v>
+      </c>
+      <c r="S5">
+        <v>849</v>
+      </c>
+      <c r="T5">
+        <v>1934.74</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>27.358490566037698</v>
+      </c>
+      <c r="X5">
+        <v>7.4766355140186898</v>
+      </c>
+      <c r="Y5">
+        <v>30.172413793103399</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1960.39</v>
+      </c>
+      <c r="AC5">
+        <v>796.96</v>
+      </c>
+      <c r="AD5">
+        <v>1196.92</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>19.780219780219799</v>
+      </c>
+      <c r="D6">
+        <v>15.0537634408602</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>1439.74</v>
+      </c>
+      <c r="I6">
+        <v>1474.4</v>
+      </c>
+      <c r="J6">
+        <v>856.26</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>16.6666666666667</v>
+      </c>
+      <c r="N6">
+        <v>15.068493150684899</v>
+      </c>
+      <c r="O6">
+        <v>36.363636363636402</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>382.61</v>
+      </c>
+      <c r="S6">
+        <v>1175</v>
+      </c>
+      <c r="T6">
+        <v>2055.98</v>
+      </c>
+      <c r="V6">
+        <v>2</v>
+      </c>
+      <c r="W6">
+        <v>16.129032258064498</v>
+      </c>
+      <c r="X6">
+        <v>11.9402985074627</v>
+      </c>
+      <c r="Y6">
+        <v>39.743589743589702</v>
+      </c>
+      <c r="AA6">
+        <v>2</v>
+      </c>
+      <c r="AB6">
+        <v>482.63</v>
+      </c>
+      <c r="AC6">
+        <v>844</v>
+      </c>
+      <c r="AD6">
+        <v>2293.67</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>30.1075268817204</v>
+      </c>
+      <c r="D7">
+        <v>15.4639175257732</v>
+      </c>
+      <c r="E7">
+        <v>6.6666666666666696</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>1728.6</v>
+      </c>
+      <c r="I7">
+        <v>1594</v>
+      </c>
+      <c r="J7">
+        <v>337.97</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>19.696969696969699</v>
+      </c>
+      <c r="N7">
+        <v>14.285714285714301</v>
+      </c>
+      <c r="O7">
+        <v>37.5</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>698.65</v>
+      </c>
+      <c r="S7">
+        <v>1052.3599999999999</v>
+      </c>
+      <c r="T7">
+        <v>1778.74</v>
+      </c>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>16.883116883116902</v>
+      </c>
+      <c r="X7">
+        <v>6.0975609756097597</v>
+      </c>
+      <c r="Y7">
+        <v>38.8888888888889</v>
+      </c>
+      <c r="AA7">
+        <v>3</v>
+      </c>
+      <c r="AB7">
+        <v>425.39</v>
+      </c>
+      <c r="AC7">
+        <v>516.21</v>
+      </c>
+      <c r="AD7">
+        <v>2621.77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>32.911392405063303</v>
+      </c>
+      <c r="D8">
+        <v>12.1951219512195</v>
+      </c>
+      <c r="E8">
+        <v>31.868131868131901</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>2017.33</v>
+      </c>
+      <c r="I8">
+        <v>1059</v>
+      </c>
+      <c r="J8">
+        <v>820.56</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>20.481927710843401</v>
+      </c>
+      <c r="N8">
+        <v>15.294117647058799</v>
+      </c>
+      <c r="O8">
+        <v>37.634408602150501</v>
+      </c>
+      <c r="Q8">
+        <v>4</v>
+      </c>
+      <c r="R8">
+        <v>747.69</v>
+      </c>
+      <c r="S8">
+        <v>1337.06</v>
+      </c>
+      <c r="T8">
+        <v>1470.48</v>
+      </c>
+      <c r="V8">
+        <v>4</v>
+      </c>
+      <c r="W8">
+        <v>13.846153846153801</v>
+      </c>
+      <c r="X8">
+        <v>16.901408450704199</v>
+      </c>
+      <c r="Y8">
+        <v>35</v>
+      </c>
+      <c r="AA8">
+        <v>4</v>
+      </c>
+      <c r="AB8">
+        <v>312.47000000000003</v>
+      </c>
+      <c r="AC8">
+        <v>1276.6300000000001</v>
+      </c>
+      <c r="AD8">
+        <v>2020.11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>21.428571428571399</v>
+      </c>
+      <c r="D9">
+        <v>15.909090909090899</v>
+      </c>
+      <c r="E9">
+        <v>34.042553191489397</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>1088.4000000000001</v>
+      </c>
+      <c r="I9">
+        <v>1489.48</v>
+      </c>
+      <c r="J9">
+        <v>1125.48</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>28.205128205128201</v>
+      </c>
+      <c r="N9">
+        <v>15.116279069767399</v>
+      </c>
+      <c r="O9">
+        <v>32.6086956521739</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9">
+        <v>1491.12</v>
+      </c>
+      <c r="S9">
+        <v>1368.43</v>
+      </c>
+      <c r="T9">
+        <v>1047.07</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="W9">
+        <v>28.8888888888889</v>
+      </c>
+      <c r="X9">
+        <v>15.2173913043478</v>
+      </c>
+      <c r="Y9">
+        <v>29.126213592233</v>
+      </c>
+      <c r="AA9">
+        <v>5</v>
+      </c>
+      <c r="AB9">
+        <v>1580.17</v>
+      </c>
+      <c r="AC9">
+        <v>1469.02</v>
+      </c>
+      <c r="AD9">
+        <v>800.56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>15.2173913043478</v>
+      </c>
+      <c r="E10">
+        <v>32.673267326732699</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>1223.73</v>
+      </c>
+      <c r="I10">
+        <v>1464.09</v>
+      </c>
+      <c r="J10">
+        <v>1106.28</v>
+      </c>
+      <c r="L10">
+        <v>6</v>
+      </c>
+      <c r="M10">
+        <v>28.571428571428601</v>
+      </c>
+      <c r="N10">
+        <v>4.1237113402061896</v>
+      </c>
+      <c r="O10">
+        <v>37.142857142857103</v>
+      </c>
+      <c r="Q10">
+        <v>6</v>
+      </c>
+      <c r="R10">
+        <v>1910.56</v>
+      </c>
+      <c r="S10">
+        <v>414.36</v>
+      </c>
+      <c r="T10">
+        <v>1588.11</v>
+      </c>
+      <c r="V10">
+        <v>6</v>
+      </c>
+      <c r="W10">
+        <v>17.0731707317073</v>
+      </c>
+      <c r="X10">
+        <v>6.7415730337078701</v>
+      </c>
+      <c r="Y10">
+        <v>37.113402061855702</v>
+      </c>
+      <c r="AA10">
+        <v>6</v>
+      </c>
+      <c r="AB10">
+        <v>418.52</v>
+      </c>
+      <c r="AC10">
+        <v>622.44000000000096</v>
+      </c>
+      <c r="AD10">
+        <v>2548.67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>24.705882352941199</v>
+      </c>
+      <c r="D11">
+        <v>15.384615384615399</v>
+      </c>
+      <c r="E11">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>1109.2</v>
+      </c>
+      <c r="I11">
+        <v>1488</v>
+      </c>
+      <c r="J11">
+        <v>1055.42</v>
+      </c>
+      <c r="L11">
+        <v>7</v>
+      </c>
+      <c r="M11">
+        <v>16.455696202531598</v>
+      </c>
+      <c r="N11">
+        <v>13.4146341463415</v>
+      </c>
+      <c r="O11">
+        <v>29.6703296703297</v>
+      </c>
+      <c r="Q11">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>574.52</v>
+      </c>
+      <c r="S11">
+        <v>1155.45</v>
+      </c>
+      <c r="T11">
+        <v>2057.0100000000002</v>
+      </c>
+      <c r="V11">
+        <v>7</v>
+      </c>
+      <c r="W11">
+        <v>11.764705882352899</v>
+      </c>
+      <c r="X11">
+        <v>13.8888888888889</v>
+      </c>
+      <c r="Y11">
+        <v>41.25</v>
+      </c>
+      <c r="AA11">
+        <v>7</v>
+      </c>
+      <c r="AB11">
+        <v>202.64</v>
+      </c>
+      <c r="AC11">
+        <v>1067</v>
+      </c>
+      <c r="AD11">
+        <v>2644.39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>8</v>
       </c>
-      <c r="N4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R4" t="s">
-        <v>0</v>
-      </c>
-      <c r="S4" t="s">
-        <v>2</v>
-      </c>
-      <c r="T4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U4" t="s">
-        <v>4</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="C12">
+        <v>21.951219512195099</v>
+      </c>
+      <c r="D12">
+        <v>18.0722891566265</v>
+      </c>
+      <c r="E12">
+        <v>36.842105263157897</v>
+      </c>
+      <c r="G12">
         <v>8</v>
       </c>
-      <c r="X4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>4</v>
+      <c r="H12">
+        <v>935.17</v>
+      </c>
+      <c r="I12">
+        <v>1582.45</v>
+      </c>
+      <c r="J12">
+        <v>1168.5</v>
+      </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>25.714285714285701</v>
+      </c>
+      <c r="N12">
+        <v>16.901408450704199</v>
+      </c>
+      <c r="O12">
+        <v>20.731707317073202</v>
+      </c>
+      <c r="Q12">
+        <v>8</v>
+      </c>
+      <c r="R12">
+        <v>1145.46</v>
+      </c>
+      <c r="S12">
+        <v>1286</v>
+      </c>
+      <c r="T12">
+        <v>1499.76</v>
+      </c>
+      <c r="V12">
+        <v>8</v>
+      </c>
+      <c r="W12">
+        <v>23.529411764705898</v>
+      </c>
+      <c r="X12">
+        <v>17.045454545454501</v>
+      </c>
+      <c r="Y12">
+        <v>33.684210526315802</v>
+      </c>
+      <c r="AA12">
+        <v>8</v>
+      </c>
+      <c r="AB12">
+        <v>790.17</v>
+      </c>
+      <c r="AC12">
+        <v>1581.79</v>
+      </c>
+      <c r="AD12">
+        <v>1310.33</v>
       </c>
     </row>
-    <row r="5" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>15.492957746478901</v>
-      </c>
-      <c r="E5">
-        <v>14.6666666666667</v>
-      </c>
-      <c r="F5">
-        <v>29.268292682926798</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>404.72</v>
-      </c>
-      <c r="J5">
-        <v>1163.02</v>
-      </c>
-      <c r="K5">
-        <v>2007.96</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>17.741935483871</v>
-      </c>
-      <c r="O5">
-        <v>11.5942028985507</v>
-      </c>
-      <c r="P5">
-        <v>35.064935064935099</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>682.19</v>
-      </c>
-      <c r="T5">
-        <v>849</v>
-      </c>
-      <c r="U5">
-        <v>1934.74</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="X5">
-        <v>27.358490566037698</v>
-      </c>
-      <c r="Y5">
-        <v>7.4766355140186898</v>
-      </c>
-      <c r="Z5">
-        <v>30.172413793103399</v>
-      </c>
-      <c r="AB5">
-        <v>1</v>
-      </c>
-      <c r="AC5">
-        <v>682.19</v>
-      </c>
-      <c r="AD5">
-        <v>849</v>
-      </c>
-      <c r="AE5">
-        <v>1934.74</v>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>18.571428571428601</v>
+      </c>
+      <c r="D13">
+        <v>17.5675675675676</v>
+      </c>
+      <c r="E13">
+        <v>33.75</v>
+      </c>
+      <c r="G13">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>400.62</v>
+      </c>
+      <c r="I13">
+        <v>1391</v>
+      </c>
+      <c r="J13">
+        <v>1907.24</v>
+      </c>
+      <c r="L13">
+        <v>9</v>
+      </c>
+      <c r="M13">
+        <v>31.645569620253202</v>
+      </c>
+      <c r="N13">
+        <v>12.048192771084301</v>
+      </c>
+      <c r="O13">
+        <v>35.869565217391298</v>
+      </c>
+      <c r="Q13">
+        <v>9</v>
+      </c>
+      <c r="R13">
+        <v>1987.18</v>
+      </c>
+      <c r="S13">
+        <v>1056.45</v>
+      </c>
+      <c r="T13">
+        <v>937.93</v>
+      </c>
+      <c r="V13">
+        <v>9</v>
+      </c>
+      <c r="W13">
+        <v>30.769230769230798</v>
+      </c>
+      <c r="X13">
+        <v>15.0537634408602</v>
+      </c>
+      <c r="Y13">
+        <v>18.269230769230798</v>
+      </c>
+      <c r="AA13">
+        <v>9</v>
+      </c>
+      <c r="AB13">
+        <v>1828.27</v>
+      </c>
+      <c r="AC13">
+        <v>1443.65</v>
+      </c>
+      <c r="AD13">
+        <v>334.67</v>
       </c>
     </row>
-    <row r="6" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>19.780219780219799</v>
-      </c>
-      <c r="E6">
-        <v>15.0537634408602</v>
-      </c>
-      <c r="F6">
-        <v>32</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>1439.74</v>
-      </c>
-      <c r="J6">
-        <v>1474.4</v>
-      </c>
-      <c r="K6">
-        <v>856.26</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-      <c r="N6">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>11.4285714285714</v>
+      </c>
+      <c r="D14">
         <v>16.6666666666667</v>
       </c>
-      <c r="O6">
-        <v>15.068493150684899</v>
-      </c>
-      <c r="P6">
-        <v>36.363636363636402</v>
-      </c>
-      <c r="R6">
-        <v>2</v>
-      </c>
-      <c r="S6">
-        <v>382.61</v>
-      </c>
-      <c r="T6">
-        <v>1175</v>
-      </c>
-      <c r="U6">
-        <v>2055.98</v>
-      </c>
-      <c r="W6">
-        <v>2</v>
-      </c>
-      <c r="X6">
-        <v>16.129032258064498</v>
-      </c>
-      <c r="Y6">
-        <v>11.9402985074627</v>
-      </c>
-      <c r="Z6">
-        <v>39.743589743589702</v>
-      </c>
-      <c r="AB6">
-        <v>2</v>
-      </c>
-      <c r="AC6">
-        <v>382.61</v>
-      </c>
-      <c r="AD6">
-        <v>1175</v>
-      </c>
-      <c r="AE6">
-        <v>2055.98</v>
-      </c>
-    </row>
-    <row r="7" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>30.1075268817204</v>
-      </c>
-      <c r="E7">
-        <v>15.4639175257732</v>
-      </c>
-      <c r="F7">
-        <v>6.6666666666666696</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <v>1728.6</v>
-      </c>
-      <c r="J7">
-        <v>1594</v>
-      </c>
-      <c r="K7">
-        <v>337.97</v>
-      </c>
-      <c r="M7">
-        <v>3</v>
-      </c>
-      <c r="N7">
-        <v>19.696969696969699</v>
-      </c>
-      <c r="O7">
-        <v>14.285714285714301</v>
-      </c>
-      <c r="P7">
-        <v>37.5</v>
-      </c>
-      <c r="R7">
-        <v>3</v>
-      </c>
-      <c r="S7">
-        <v>698.65</v>
-      </c>
-      <c r="T7">
-        <v>1052.3599999999999</v>
-      </c>
-      <c r="U7">
-        <v>1778.74</v>
-      </c>
-      <c r="W7">
-        <v>3</v>
-      </c>
-      <c r="X7">
-        <v>16.883116883116902</v>
-      </c>
-      <c r="Y7">
-        <v>6.0975609756097597</v>
-      </c>
-      <c r="Z7">
-        <v>38.8888888888889</v>
-      </c>
-      <c r="AB7">
-        <v>3</v>
-      </c>
-      <c r="AC7">
-        <v>698.65</v>
-      </c>
-      <c r="AD7">
-        <v>1052.3599999999999</v>
-      </c>
-      <c r="AE7">
-        <v>1778.74</v>
-      </c>
-    </row>
-    <row r="8" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>32.911392405063303</v>
-      </c>
-      <c r="E8">
-        <v>12.1951219512195</v>
-      </c>
-      <c r="F8">
-        <v>31.868131868131901</v>
-      </c>
-      <c r="H8">
-        <v>4</v>
-      </c>
-      <c r="I8">
-        <v>2017.33</v>
-      </c>
-      <c r="J8">
-        <v>1059</v>
-      </c>
-      <c r="K8">
-        <v>820.56</v>
-      </c>
-      <c r="M8">
-        <v>4</v>
-      </c>
-      <c r="N8">
-        <v>20.481927710843401</v>
-      </c>
-      <c r="O8">
-        <v>15.294117647058799</v>
-      </c>
-      <c r="P8">
-        <v>37.634408602150501</v>
-      </c>
-      <c r="R8">
-        <v>4</v>
-      </c>
-      <c r="S8">
-        <v>747.69</v>
-      </c>
-      <c r="T8">
-        <v>1337.06</v>
-      </c>
-      <c r="U8">
-        <v>1470.48</v>
-      </c>
-      <c r="W8">
-        <v>4</v>
-      </c>
-      <c r="X8">
-        <v>13.846153846153801</v>
-      </c>
-      <c r="Y8">
-        <v>16.901408450704199</v>
-      </c>
-      <c r="Z8">
-        <v>35</v>
-      </c>
-      <c r="AB8">
-        <v>4</v>
-      </c>
-      <c r="AC8">
-        <v>747.69</v>
-      </c>
-      <c r="AD8">
-        <v>1337.06</v>
-      </c>
-      <c r="AE8">
-        <v>1470.48</v>
-      </c>
-    </row>
-    <row r="9" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>21.428571428571399</v>
-      </c>
-      <c r="E9">
-        <v>15.909090909090899</v>
-      </c>
-      <c r="F9">
-        <v>34.042553191489397</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="I9">
-        <v>1088.4000000000001</v>
-      </c>
-      <c r="J9">
-        <v>1489.48</v>
-      </c>
-      <c r="K9">
-        <v>1125.48</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
-      <c r="N9">
-        <v>28.205128205128201</v>
-      </c>
-      <c r="O9">
-        <v>15.116279069767399</v>
-      </c>
-      <c r="P9">
-        <v>32.6086956521739</v>
-      </c>
-      <c r="R9">
-        <v>5</v>
-      </c>
-      <c r="S9">
-        <v>1491.12</v>
-      </c>
-      <c r="T9">
-        <v>1368.43</v>
-      </c>
-      <c r="U9">
-        <v>1047.07</v>
-      </c>
-      <c r="W9">
-        <v>5</v>
-      </c>
-      <c r="X9">
-        <v>28.8888888888889</v>
-      </c>
-      <c r="Y9">
-        <v>15.2173913043478</v>
-      </c>
-      <c r="Z9">
-        <v>29.126213592233</v>
-      </c>
-      <c r="AB9">
-        <v>5</v>
-      </c>
-      <c r="AC9">
-        <v>1491.12</v>
-      </c>
-      <c r="AD9">
-        <v>1368.43</v>
-      </c>
-      <c r="AE9">
-        <v>1047.07</v>
-      </c>
-    </row>
-    <row r="10" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
-        <v>15.2173913043478</v>
-      </c>
-      <c r="F10">
-        <v>32.673267326732699</v>
-      </c>
-      <c r="H10">
-        <v>6</v>
-      </c>
-      <c r="I10">
-        <v>1223.73</v>
-      </c>
-      <c r="J10">
-        <v>1464.09</v>
-      </c>
-      <c r="K10">
-        <v>1106.28</v>
-      </c>
-      <c r="M10">
-        <v>6</v>
-      </c>
-      <c r="N10">
-        <v>28.571428571428601</v>
-      </c>
-      <c r="O10">
-        <v>4.1237113402061896</v>
-      </c>
-      <c r="P10">
-        <v>37.142857142857103</v>
-      </c>
-      <c r="R10">
-        <v>6</v>
-      </c>
-      <c r="S10">
-        <v>1910.56</v>
-      </c>
-      <c r="T10">
-        <v>414.36</v>
-      </c>
-      <c r="U10">
-        <v>1588.11</v>
-      </c>
-      <c r="W10">
-        <v>6</v>
-      </c>
-      <c r="X10">
-        <v>17.0731707317073</v>
-      </c>
-      <c r="Y10">
-        <v>6.7415730337078701</v>
-      </c>
-      <c r="Z10">
+      <c r="E14">
+        <v>27.380952380952401</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>326.02999999999997</v>
+      </c>
+      <c r="I14">
+        <v>1396.81</v>
+      </c>
+      <c r="J14">
+        <v>1716.02</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>20.2247191011236</v>
+      </c>
+      <c r="N14">
+        <v>13.483146067415699</v>
+      </c>
+      <c r="O14">
+        <v>43.137254901960802</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>907.07</v>
+      </c>
+      <c r="S14">
+        <v>1262.81</v>
+      </c>
+      <c r="T14">
+        <v>1588.05</v>
+      </c>
+      <c r="V14">
+        <v>10</v>
+      </c>
+      <c r="W14">
+        <v>25.882352941176499</v>
+      </c>
+      <c r="X14">
+        <v>11.363636363636401</v>
+      </c>
+      <c r="Y14">
         <v>37.113402061855702</v>
       </c>
-      <c r="AB10">
-        <v>6</v>
-      </c>
-      <c r="AC10">
-        <v>1910.56</v>
-      </c>
-      <c r="AD10">
-        <v>414.36</v>
-      </c>
-      <c r="AE10">
-        <v>1588.11</v>
-      </c>
-    </row>
-    <row r="11" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>24.705882352941199</v>
-      </c>
-      <c r="E11">
-        <v>15.384615384615399</v>
-      </c>
-      <c r="F11">
-        <v>32</v>
-      </c>
-      <c r="H11">
-        <v>7</v>
-      </c>
-      <c r="I11">
-        <v>1109.2</v>
-      </c>
-      <c r="J11">
-        <v>1488</v>
-      </c>
-      <c r="K11">
-        <v>1055.42</v>
-      </c>
-      <c r="M11">
-        <v>7</v>
-      </c>
-      <c r="N11">
-        <v>16.455696202531598</v>
-      </c>
-      <c r="O11">
-        <v>13.4146341463415</v>
-      </c>
-      <c r="P11">
-        <v>29.6703296703297</v>
-      </c>
-      <c r="R11">
-        <v>7</v>
-      </c>
-      <c r="S11">
-        <v>574.52</v>
-      </c>
-      <c r="T11">
-        <v>1155.45</v>
-      </c>
-      <c r="U11">
-        <v>2057.0100000000002</v>
-      </c>
-      <c r="W11">
-        <v>7</v>
-      </c>
-      <c r="X11">
-        <v>11.764705882352899</v>
-      </c>
-      <c r="Y11">
-        <v>13.8888888888889</v>
-      </c>
-      <c r="Z11">
-        <v>41.25</v>
-      </c>
-      <c r="AB11">
-        <v>7</v>
-      </c>
-      <c r="AC11">
-        <v>574.52</v>
-      </c>
-      <c r="AD11">
-        <v>1155.45</v>
-      </c>
-      <c r="AE11">
-        <v>2057.0100000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>21.951219512195099</v>
-      </c>
-      <c r="E12">
-        <v>18.0722891566265</v>
-      </c>
-      <c r="F12">
-        <v>36.842105263157897</v>
-      </c>
-      <c r="H12">
-        <v>8</v>
-      </c>
-      <c r="I12">
-        <v>935.17</v>
-      </c>
-      <c r="J12">
-        <v>1582.45</v>
-      </c>
-      <c r="K12">
-        <v>1168.5</v>
-      </c>
-      <c r="M12">
-        <v>8</v>
-      </c>
-      <c r="N12">
-        <v>25.714285714285701</v>
-      </c>
-      <c r="O12">
-        <v>16.901408450704199</v>
-      </c>
-      <c r="P12">
-        <v>20.731707317073202</v>
-      </c>
-      <c r="R12">
-        <v>8</v>
-      </c>
-      <c r="S12">
-        <v>1145.46</v>
-      </c>
-      <c r="T12">
-        <v>1286</v>
-      </c>
-      <c r="U12">
-        <v>1499.76</v>
-      </c>
-      <c r="W12">
-        <v>8</v>
-      </c>
-      <c r="X12">
-        <v>23.529411764705898</v>
-      </c>
-      <c r="Y12">
-        <v>17.045454545454501</v>
-      </c>
-      <c r="Z12">
-        <v>33.684210526315802</v>
-      </c>
-      <c r="AB12">
-        <v>8</v>
-      </c>
-      <c r="AC12">
-        <v>1145.46</v>
-      </c>
-      <c r="AD12">
-        <v>1286</v>
-      </c>
-      <c r="AE12">
-        <v>1499.76</v>
-      </c>
-    </row>
-    <row r="13" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <v>18.571428571428601</v>
-      </c>
-      <c r="E13">
-        <v>17.5675675675676</v>
-      </c>
-      <c r="F13">
-        <v>33.75</v>
-      </c>
-      <c r="H13">
-        <v>9</v>
-      </c>
-      <c r="I13">
-        <v>400.62</v>
-      </c>
-      <c r="J13">
-        <v>1391</v>
-      </c>
-      <c r="K13">
-        <v>1907.24</v>
-      </c>
-      <c r="M13">
-        <v>9</v>
-      </c>
-      <c r="N13">
-        <v>31.645569620253202</v>
-      </c>
-      <c r="O13">
-        <v>12.048192771084301</v>
-      </c>
-      <c r="P13">
-        <v>35.869565217391298</v>
-      </c>
-      <c r="R13">
-        <v>9</v>
-      </c>
-      <c r="S13">
-        <v>1987.18</v>
-      </c>
-      <c r="T13">
-        <v>1056.45</v>
-      </c>
-      <c r="U13">
-        <v>937.93</v>
-      </c>
-      <c r="W13">
-        <v>9</v>
-      </c>
-      <c r="X13">
-        <v>30.769230769230798</v>
-      </c>
-      <c r="Y13">
-        <v>15.0537634408602</v>
-      </c>
-      <c r="Z13">
-        <v>18.269230769230798</v>
-      </c>
-      <c r="AB13">
-        <v>9</v>
-      </c>
-      <c r="AC13">
-        <v>1987.18</v>
-      </c>
-      <c r="AD13">
-        <v>1056.45</v>
-      </c>
-      <c r="AE13">
-        <v>937.93</v>
-      </c>
-    </row>
-    <row r="14" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C14">
+      <c r="AA14">
         <v>10</v>
       </c>
-      <c r="D14">
-        <v>11.4285714285714</v>
-      </c>
-      <c r="E14">
-        <v>16.6666666666667</v>
-      </c>
-      <c r="F14">
-        <v>27.380952380952401</v>
-      </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
-      <c r="I14">
-        <v>326.02999999999997</v>
-      </c>
-      <c r="J14">
-        <v>1396.81</v>
-      </c>
-      <c r="K14">
-        <v>1716.02</v>
-      </c>
-      <c r="M14">
-        <v>10</v>
-      </c>
-      <c r="N14">
-        <v>20.2247191011236</v>
-      </c>
-      <c r="O14">
-        <v>13.483146067415699</v>
-      </c>
-      <c r="P14">
-        <v>43.137254901960802</v>
-      </c>
-      <c r="R14">
-        <v>10</v>
-      </c>
-      <c r="S14">
-        <v>907.07</v>
-      </c>
-      <c r="T14">
-        <v>1262.81</v>
-      </c>
-      <c r="U14">
-        <v>1588.05</v>
-      </c>
-      <c r="W14">
-        <v>10</v>
-      </c>
-      <c r="X14">
-        <v>25.882352941176499</v>
-      </c>
-      <c r="Y14">
-        <v>11.363636363636401</v>
-      </c>
-      <c r="Z14">
-        <v>37.113402061855702</v>
-      </c>
       <c r="AB14">
-        <v>10</v>
+        <v>1347.6</v>
       </c>
       <c r="AC14">
-        <v>907.07</v>
+        <v>1057</v>
       </c>
       <c r="AD14">
-        <v>1262.81</v>
-      </c>
-      <c r="AE14">
-        <v>1588.05</v>
+        <v>1169.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>